<commit_message>
Clean up on emp table
</commit_message>
<xml_diff>
--- a/sample_csv/emp_all_data.xlsx
+++ b/sample_csv/emp_all_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raghuvallikkat/Desktop/LEADSOC_CODE/CRM1.0/sample_csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E580F06-60CA-4548-BF7E-CFF4B311E79D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F79BE9-B6FF-5B4B-97C6-A52CFF730534}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="3600" windowWidth="28320" windowHeight="11940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="109">
   <si>
     <t>Employee ID</t>
   </si>
@@ -97,9 +97,6 @@
     <t>suresh@gmail.com</t>
   </si>
   <si>
-    <t>C,C++</t>
-  </si>
-  <si>
     <t>Deployed</t>
   </si>
   <si>
@@ -347,6 +344,12 @@
   </si>
   <si>
     <t>VM</t>
+  </si>
+  <si>
+    <t>project Management</t>
+  </si>
+  <si>
+    <t>yaseen</t>
   </si>
 </sst>
 </file>
@@ -753,7 +756,7 @@
   <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -810,16 +813,16 @@
         <v>11</v>
       </c>
       <c r="M1" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="N1" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="O1" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="O1" s="9" t="s">
-        <v>72</v>
-      </c>
       <c r="P1" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -860,16 +863,16 @@
         <v>45051</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O2" t="b">
         <v>0</v>
       </c>
       <c r="P2" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -882,8 +885,8 @@
       <c r="C3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
+      <c r="D3" s="9" t="s">
+        <v>50</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>23</v>
@@ -895,13 +898,13 @@
         <v>5</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>24</v>
+        <v>107</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="K3" s="8">
         <v>45028</v>
@@ -910,13 +913,13 @@
         <v>45058</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="O3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P3" s="9" t="s">
         <v>82</v>
@@ -924,19 +927,19 @@
     </row>
     <row r="4" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="F4" s="6">
         <v>8769457112</v>
@@ -945,13 +948,13 @@
         <v>4</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="J4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K4" s="8">
         <v>45031</v>
@@ -960,33 +963,33 @@
         <v>45063</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O4" t="b">
         <v>0</v>
       </c>
       <c r="P4" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F5" s="6">
         <v>9758648113</v>
@@ -995,7 +998,7 @@
         <v>5</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>18</v>
@@ -1010,33 +1013,33 @@
         <v>45063</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O5" t="b">
         <v>0</v>
       </c>
       <c r="P5" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="F6" s="6">
         <v>8971234114</v>
@@ -1045,10 +1048,10 @@
         <v>4</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>19</v>
@@ -1060,33 +1063,33 @@
         <v>45060</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O6" t="b">
         <v>1</v>
       </c>
       <c r="P6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="F7" s="6">
         <v>8975647115</v>
@@ -1095,7 +1098,7 @@
         <v>4</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>18</v>
@@ -1110,33 +1113,33 @@
         <v>45061</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O7" t="b">
         <v>0</v>
       </c>
       <c r="P7" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>52</v>
       </c>
       <c r="F8" s="6">
         <v>8722331155</v>
@@ -1146,10 +1149,10 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="K8" s="8">
         <v>45058</v>
@@ -1158,33 +1161,33 @@
         <v>45061</v>
       </c>
       <c r="M8" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O8" t="b">
         <v>1</v>
       </c>
       <c r="P8" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="F9" s="6">
         <v>1</v>
@@ -1193,13 +1196,13 @@
         <v>4</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="K9" s="8">
         <v>45058</v>
@@ -1208,33 +1211,33 @@
         <v>45061</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O9" t="b">
         <v>1</v>
       </c>
       <c r="P9" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>62</v>
       </c>
       <c r="F10" s="6">
         <v>2</v>
@@ -1244,10 +1247,10 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K10" s="8">
         <v>45058</v>
@@ -1256,33 +1259,33 @@
         <v>45061</v>
       </c>
       <c r="M10" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="O10" t="b">
         <v>0</v>
       </c>
       <c r="P10" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>66</v>
       </c>
       <c r="F11" s="6">
         <v>3</v>
@@ -1292,10 +1295,10 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K11" s="8">
         <v>45058</v>
@@ -1304,33 +1307,33 @@
         <v>45061</v>
       </c>
       <c r="M11" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="O11" t="b">
         <v>0</v>
       </c>
       <c r="P11" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="F12" s="6">
         <v>4</v>
@@ -1339,13 +1342,13 @@
         <v>4</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K12" s="8">
         <v>45058</v>
@@ -1354,33 +1357,33 @@
         <v>45061</v>
       </c>
       <c r="M12" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O12" t="b">
         <v>1</v>
       </c>
       <c r="P12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F13" s="6">
         <v>5</v>
@@ -1389,13 +1392,13 @@
         <v>4</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K13" s="8">
         <v>45058</v>
@@ -1404,33 +1407,33 @@
         <v>45061</v>
       </c>
       <c r="M13" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="O13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F14" s="6">
         <v>6</v>
@@ -1439,13 +1442,13 @@
         <v>4</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K14" s="8">
         <v>45058</v>
@@ -1454,33 +1457,33 @@
         <v>45061</v>
       </c>
       <c r="M14" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P14" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F15" s="6">
         <v>7</v>
@@ -1489,13 +1492,13 @@
         <v>4</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K15" s="8">
         <v>45058</v>
@@ -1504,33 +1507,33 @@
         <v>45061</v>
       </c>
       <c r="M15" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N15" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P15" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="B16" s="9" t="s">
-        <v>96</v>
-      </c>
       <c r="C16" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F16" s="6">
         <v>8</v>
@@ -1539,13 +1542,13 @@
         <v>4</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K16" s="8">
         <v>45058</v>
@@ -1554,33 +1557,33 @@
         <v>45061</v>
       </c>
       <c r="M16" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O16" t="b">
         <v>1</v>
       </c>
       <c r="P16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="B17" s="9" t="s">
-        <v>98</v>
-      </c>
       <c r="C17" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F17" s="6">
         <v>9</v>
@@ -1589,13 +1592,13 @@
         <v>4</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K17" s="8">
         <v>45058</v>
@@ -1604,33 +1607,33 @@
         <v>45061</v>
       </c>
       <c r="M17" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O17" t="b">
         <v>1</v>
       </c>
       <c r="P17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>100</v>
-      </c>
       <c r="C18" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F18" s="6">
         <v>10</v>
@@ -1639,13 +1642,13 @@
         <v>4</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K18" s="8">
         <v>45058</v>
@@ -1654,16 +1657,16 @@
         <v>45061</v>
       </c>
       <c r="M18" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="O18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>